<commit_message>
Revision folders et assets
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bfarg\Desktop\TradingView.Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17B7039-5DAE-424E-9B60-40F09C7B8F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BC9E8E-252A-4EF0-9BF8-ADD90EE71086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,18 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Bfa.00</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Exchange</t>
   </si>
   <si>
+    <t>b.fargeout@outlook.com</t>
+  </si>
+  <si>
     <t>ByBit</t>
   </si>
   <si>
-    <t>Id</t>
+    <t>User</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>BFA.BB01.Dev</t>
   </si>
 </sst>
 </file>
@@ -80,11 +86,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,29 +370,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" customWidth="1"/>
-    <col min="2" max="2" width="12.9296875" customWidth="1"/>
+    <col min="1" max="1" width="12.73046875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.46484375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.06640625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>